<commit_message>
2SLS on NUTS 2 analysis + gitignore
</commit_message>
<xml_diff>
--- a/raw_data/eurostat/nuts2_emp_sbs_9507.xlsx
+++ b/raw_data/eurostat/nuts2_emp_sbs_9507.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aml/AutoEmp/raw_data/eurostat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3850DD13-F2AF-2E4D-A754-9E737E42BA55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A1F065-F92F-414F-901F-FFBC5FB7C5EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40717,11 +40717,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:T93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="11" topLeftCell="C55" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="2" ySplit="11" topLeftCell="J23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N71" sqref="N71"/>
+      <selection pane="bottomRight" activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>